<commit_message>
Update the template constant
</commit_message>
<xml_diff>
--- a/app/core/template_constant.xlsx
+++ b/app/core/template_constant.xlsx
@@ -354,7 +354,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>air kerma rate</t>
+    <t>Nominal air kerma rate</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2316,7 +2316,7 @@
   <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>